<commit_message>
tested and corrected some errors
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nike Inc</t>
+          <t>Coca-Cola Company The</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$67.94</t>
+          <t>$68.67</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-3.92(5.46%) 1D</t>
+          <t>-1.04(1.49%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -494,6 +494,116 @@
         </is>
       </c>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Apple Inc</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>$218.27</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>+4.17(1.95%) 1D</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>British American Tobacco plc</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>$40.83</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-0.24(0.58%) 1D</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Amazon.com Inc.</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>$196.21</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>+1.26(0.65%) 1D</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Philip Morris International Inc</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>$151.48</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>-0.99(0.65%) 1D</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NVIDIA Corporation</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>$117.70</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>-0.83(0.70%) 1D</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>

<commit_message>
added input for stock ticker
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,147 +463,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$68.67</t>
+          <t>$68.93</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-1.04(1.49%) 1D</t>
+          <t>-0.02(0.03%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Fresh Del Monte Produce Inc</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>$29.65</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-0.28(0.94%) 1D</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Apple Inc</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>$218.27</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>+4.17(1.95%) 1D</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>British American Tobacco plc</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>$40.83</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-0.24(0.58%) 1D</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Amazon.com Inc.</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>$196.21</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>+1.26(0.65%) 1D</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Philip Morris International Inc</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>$151.48</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-0.99(0.65%) 1D</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>NVIDIA Corporation</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>$117.70</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>-0.83(0.70%) 1D</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>

<commit_message>
added P/E ratio extraction
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,26 +454,36 @@
           <t>Volume</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>P_E</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Amazon.com Inc.</t>
+          <t>Coca-Cola Company The</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$204.40</t>
+          <t>$70.00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+1.14(0.56%) 1D</t>
+          <t>-0.02(0.03%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>N/A</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>28.3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added License, extraction for market cap, div yield
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,27 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Volume</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>P_E</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>EPS(TTM)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Div. Yield</t>
         </is>
       </c>
     </row>
@@ -473,27 +483,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$70.80</t>
+          <t>$70.37</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+0.06(0.08%) 1D</t>
+          <t>-0.37(0.52%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>$302.66B</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>28.6</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>28.5</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>0.71</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2.88%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added extraction for P/B ratio
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,15 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>P_B</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>EPS(TTM)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Div. Yield</t>
         </is>
@@ -478,22 +483,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Coca-Cola Company The</t>
+          <t>Philip Morris International Inc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$70.37</t>
+          <t>$155.16</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-0.37(0.52%) 1D</t>
+          <t>+0.15(0.10%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$302.66B</t>
+          <t>$241.25B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -503,17 +508,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>28.5</t>
+          <t>34.2</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>-20.5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2.88%</t>
+          <t>1.32</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>3.48%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
started refactoring code toe xtract detailed financial info
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -493,17 +493,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$70.61</t>
+          <t>$71.77</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+0.24(0.34%) 1D</t>
+          <t>+0.15(0.21%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$302.66B</t>
+          <t>$308.03B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -513,12 +513,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>28.5</t>
+          <t>29</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12.2</t>
+          <t>12.4</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -528,7 +528,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.90%</t>
+          <t>2.85%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">

</xml_diff>

<commit_message>
most of the refactoring done, added revenues extraction and better export
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>Book Value</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Revenues</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -493,17 +498,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$71.77</t>
+          <t>$72.06</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+0.15(0.21%) 1D</t>
+          <t>+0.19(0.26%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$308.03B</t>
+          <t>$309.11B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -513,7 +518,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>29.1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -528,12 +533,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.85%</t>
+          <t>2.84%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>6.09</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>10,980</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
minimal changes, experimenting with other extraction methods
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,11 @@
           <t>Revenues</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Cost of revenues</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -498,17 +503,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$72.06</t>
+          <t>$71.68</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+0.19(0.26%) 1D</t>
+          <t>+0.35(0.49%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$309.11B</t>
+          <t>$306.79B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -518,12 +523,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>29.1</t>
+          <t>28.9</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12.4</t>
+          <t>12.3</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -533,7 +538,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.84%</t>
+          <t>2.86%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -543,7 +548,12 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>10,980</t>
+          <t>11,953</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
managed to solve detailed info extraction
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Cost of revenues</t>
+          <t>Cost of Revenues</t>
         </is>
       </c>
     </row>
@@ -503,17 +503,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$71.68</t>
+          <t>$71.99</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+0.35(0.49%) 1D</t>
+          <t>-1.19(1.63%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$306.79B</t>
+          <t>$314.74B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -523,12 +523,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>28.9</t>
+          <t>29.6</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12.3</t>
+          <t>12.7</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.86%</t>
+          <t>2.79%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4,657</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
working on adding a separate line for some detailed infos in excel
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,26 @@
           <t>Cost of Revenues</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>General &amp; Administrative Expenses in USD millions</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Operating Expenses in USD millions</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Interest Expense in USD millions</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Depreciation, Amortization &amp; Accretion in USD millions</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -503,17 +523,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$71.99</t>
+          <t>$69.93</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-1.19(1.63%) 1D</t>
+          <t>-3.25(4.44%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$314.74B</t>
+          <t>$300.76B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -523,12 +543,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>29.6</t>
+          <t>28.3</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12.7</t>
+          <t>12.1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -554,6 +574,26 @@
       <c r="L2" t="inlineStr">
         <is>
           <t>4,657</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>3,667</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>4,026</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>368</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>290</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finished extraction quarterly results
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,12 +461,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>P_E</t>
+          <t>P_E ratio</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>P_B</t>
+          <t>P_B ratio</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -482,36 +482,6 @@
       <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Book Value</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Revenues</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Cost of Revenues</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>General &amp; Administrative Expenses in USD millions</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Operating Expenses in USD millions</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Interest Expense in USD millions</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Depreciation, Amortization &amp; Accretion in USD millions</t>
         </is>
       </c>
     </row>
@@ -566,34 +536,118 @@
           <t>6.09</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Revenues</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Cost of Revenues</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>General &amp; Administrative Expenses in USD millions</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>Operating Expenses in USD millions</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>Interest Expense in USD millions</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>Depreciation, Amortization &amp; Accretion in USD millions</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>EBITDA</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>Gross Profit</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
+          <t>Net Income</t>
+        </is>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>Weighted Average Shares</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>Operating Income</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>11,953</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>4,657</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>3,667</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>4,026</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>368</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>290</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>4,199</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>7,296</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>3,087</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>4,324</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>3,270</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
working on balance sheet extraction, currently not extracting data
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -651,6 +651,110 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Shareholders Equity</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>Total Assets</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>Current Assets</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>Assets Non-Current</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>Current Liabilities</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>Liabilities Non-Current</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
+          <t>Tax Liabilities</t>
+        </is>
+      </c>
+      <c r="H8" s="1" t="inlineStr">
+        <is>
+          <t>Tax Assets</t>
+        </is>
+      </c>
+      <c r="I8" s="1" t="inlineStr">
+        <is>
+          <t>Cash and Equivalents (USD)</t>
+        </is>
+      </c>
+      <c r="J8" s="1" t="inlineStr">
+        <is>
+          <t>Total Liabilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
small refactoring, balance sheet extraction still not working
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -493,12 +493,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$69.93</t>
+          <t>$67.05</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-3.25(4.44%) 1D</t>
+          <t>-2.88(4.12%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -528,7 +528,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.79%</t>
+          <t>2.92%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">

</xml_diff>

<commit_message>
resolved balance sheet extraction
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,17 +493,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$67.05</t>
+          <t>$68.69</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-2.88(4.12%) 1D</t>
+          <t>+0.32(0.47%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$300.76B</t>
+          <t>$294.05B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -513,12 +513,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>28.3</t>
+          <t>27.7</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12.1</t>
+          <t>11.8</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -528,230 +528,230 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.92%</t>
+          <t>2.98%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>6.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Revenues</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Cost of Revenues</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>General &amp; Administrative Expenses in USD millions</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>Operating Expenses in USD millions</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Interest Expense in USD millions</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>Depreciation, Amortization &amp; Accretion in USD millions</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>EBITDA</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>Gross Profit</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>Net Income</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>Weighted Average Shares</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>Operating Income</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Revenues</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>Cost of Revenues</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>General &amp; Administrative Expenses in USD millions</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>Operating Expenses in USD millions</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>Interest Expense in USD millions</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="inlineStr">
-        <is>
-          <t>Depreciation, Amortization &amp; Accretion in USD millions</t>
-        </is>
-      </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>EBITDA</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t>Gross Profit</t>
-        </is>
-      </c>
-      <c r="I5" s="1" t="inlineStr">
-        <is>
-          <t>Net Income</t>
-        </is>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>Weighted Average Shares</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>Operating Income</t>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>11,953</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4,657</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3,667</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4,026</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>368</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>290</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>4,199</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>7,296</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>3,087</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>4,324</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>3,270</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>11,953</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4,657</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>3,667</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>4,026</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>368</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>290</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>4,199</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>7,296</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>3,087</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>4,324</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>3,270</t>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Shareholders Equity</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Total Assets</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>Current Assets</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>Assets Non-Current</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>Current Liabilities</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="inlineStr">
+        <is>
+          <t>Liabilities Non-Current</t>
+        </is>
+      </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>Tax Liabilities</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="inlineStr">
+        <is>
+          <t>Tax Assets</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>Cash and Equivalents (USD)</t>
+        </is>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>Total Liabilities</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Shareholders Equity</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>Total Assets</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>Current Assets</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>Assets Non-Current</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>Current Liabilities</t>
-        </is>
-      </c>
-      <c r="F8" s="1" t="inlineStr">
-        <is>
-          <t>Liabilities Non-Current</t>
-        </is>
-      </c>
-      <c r="G8" s="1" t="inlineStr">
-        <is>
-          <t>Tax Liabilities</t>
-        </is>
-      </c>
-      <c r="H8" s="1" t="inlineStr">
-        <is>
-          <t>Tax Assets</t>
-        </is>
-      </c>
-      <c r="I8" s="1" t="inlineStr">
-        <is>
-          <t>Cash and Equivalents (USD)</t>
-        </is>
-      </c>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t>Total Liabilities</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>N/A</t>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>24,105</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>92,763</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>22,591</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>70,172</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>19,724</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>47,213</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>4,117</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1,746</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>10,562</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>66,937</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added cash flow extraction
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,17 +493,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$71.16</t>
+          <t>$71.43</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+0.40(0.57%) 1D</t>
+          <t>+0.67(0.95%) 1D</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$304.33B</t>
+          <t>$307.22B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -513,12 +513,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>28.6</t>
+          <t>28.9</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12.2</t>
+          <t>12.4</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -752,6 +752,110 @@
       <c r="J8" t="inlineStr">
         <is>
           <t>66,937</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Investing Cash Flow</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>Operations Cash Flow</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>Financing Cash Flow</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>Net Cash Flow</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>Free Cash Flow</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="inlineStr">
+        <is>
+          <t>Capital Expenditure</t>
+        </is>
+      </c>
+      <c r="G10" s="1" t="inlineStr">
+        <is>
+          <t>Cash and Equivalents</t>
+        </is>
+      </c>
+      <c r="H10" s="1" t="inlineStr">
+        <is>
+          <t>Payments &amp; Cash Distribution</t>
+        </is>
+      </c>
+      <c r="I10" s="1" t="inlineStr">
+        <is>
+          <t>Basic Common Share</t>
+        </is>
+      </c>
+      <c r="J10" s="1" t="inlineStr">
+        <is>
+          <t>Working Capital</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>-763</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11,018</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>-10,250</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>-200</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>9,609</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-1,409</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>10,562</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-7,616</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2,867</t>
         </is>
       </c>
     </row>

</xml_diff>